<commit_message>
added bike rack and category cost breakdown
</commit_message>
<xml_diff>
--- a/myrepo/Tesla_Model_3_Loan_Analysis.xlsx
+++ b/myrepo/Tesla_Model_3_Loan_Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrw7f\github-mwyatt9214\myrepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{DD2B698A-69D6-423E-A5B5-73D6D7423D8E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65942849-CDEC-4263-A2D8-E68B6635E75B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Insurance" sheetId="5" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -450,7 +450,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="168">
   <si>
     <t>Total OutOfPocket</t>
   </si>
@@ -924,6 +924,36 @@
   </si>
   <si>
     <t>seasucker</t>
+  </si>
+  <si>
+    <t>J1772 adapter</t>
+  </si>
+  <si>
+    <t>Tesla</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Performance</t>
+  </si>
+  <si>
+    <t>Category 2</t>
+  </si>
+  <si>
+    <t>Aesthetic</t>
+  </si>
+  <si>
+    <t>Comfort</t>
+  </si>
+  <si>
+    <t>Maintenance</t>
+  </si>
+  <si>
+    <t>Efficiency</t>
+  </si>
+  <si>
+    <t>Functionality</t>
   </si>
 </sst>
 </file>
@@ -1199,6 +1229,1002 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="50" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>AfterMarket</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> by Category</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="50" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="27000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+            <a:scene3d>
+              <a:camera prst="orthographicFront"/>
+              <a:lightRig rig="threePt" dir="t"/>
+            </a:scene3d>
+            <a:sp3d prstMaterial="translucentPowder">
+              <a:contourClr>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Features!$K$8:$K$12</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Performance</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Aesthetic</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Comfort</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Functionality</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Features!$L$8:$L$12</c:f>
+              <c:numCache>
+                <c:formatCode>\$#,##0.00_);[Red]"($"#,##0.00\)</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-3387.2200000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-550</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-850</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6671-4A64-8329-11A20DD679EE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="625883384"/>
+        <c:axId val="625881088"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="625883384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="high"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="625881088"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="625881088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="\$#,##0.00_);[Red]&quot;($&quot;#,##0.00\)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="625883384"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="292">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+      <a:scene3d>
+        <a:camera prst="orthographicFront"/>
+        <a:lightRig rig="threePt" dir="t"/>
+      </a:scene3d>
+      <a:sp3d prstMaterial="translucentPowder"/>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="70000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:alpha val="27000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:sp3d/>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="0" kern="1200" cap="none" spc="50" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="15875" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:sp3d/>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1669,7 +2695,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1718,7 +2744,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1767,7 +2793,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1816,7 +2842,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1865,7 +2891,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1914,7 +2940,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1963,7 +2989,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2012,7 +3038,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2061,7 +3087,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2098,6 +3124,42 @@
         </a:ln>
       </xdr:spPr>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>5950</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>72033</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>506013</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>136327</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D52A36F2-0B21-44D2-92A4-2994C2403359}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2369,7 +3431,7 @@
   <dimension ref="A1:Q41"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2777,7 +3839,7 @@
         <v>54</v>
       </c>
       <c r="B16" s="12">
-        <f>Features!F41</f>
+        <f>Features!F42</f>
         <v>-5787.22</v>
       </c>
     </row>
@@ -3335,10 +4397,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:U41"/>
+  <dimension ref="A1:U45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="F4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3522,6 +4584,19 @@
       <c r="H8" t="s">
         <v>141</v>
       </c>
+      <c r="I8" s="39" t="s">
+        <v>160</v>
+      </c>
+      <c r="J8" s="39" t="s">
+        <v>162</v>
+      </c>
+      <c r="K8" t="s">
+        <v>161</v>
+      </c>
+      <c r="L8" s="12">
+        <f>SUMIF(I:I,"Performance",F:F)</f>
+        <v>-3387.2200000000003</v>
+      </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
@@ -3537,7 +4612,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="12">
-        <f t="shared" ref="F9:H40" si="1">IF(E9=1,D9,0)</f>
+        <f t="shared" ref="F9:H41" si="1">IF(E9=1,D9,0)</f>
         <v>0</v>
       </c>
       <c r="G9">
@@ -3546,6 +4621,19 @@
       <c r="H9" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>161</v>
+      </c>
+      <c r="J9" t="s">
+        <v>163</v>
+      </c>
+      <c r="K9" t="s">
+        <v>163</v>
+      </c>
+      <c r="L9" s="12">
+        <f>SUMIF(I:I,"Aesthetic",F:F)</f>
+        <v>-1000</v>
       </c>
     </row>
     <row r="10" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.45">
@@ -3571,6 +4659,19 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="I10" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="J10" t="s">
+        <v>163</v>
+      </c>
+      <c r="K10" t="s">
+        <v>164</v>
+      </c>
+      <c r="L10" s="12">
+        <f>SUMIF(I:I,"Comfort",F:F)</f>
+        <v>-550</v>
+      </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.45">
       <c r="C11" t="s">
@@ -3593,10 +4694,17 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I11" s="11"/>
+      <c r="I11" s="11" t="s">
+        <v>161</v>
+      </c>
       <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
+      <c r="K11" t="s">
+        <v>165</v>
+      </c>
+      <c r="L11" s="12">
+        <f>SUMIF(I:I,"Maintenance",F:F)</f>
+        <v>-850</v>
+      </c>
       <c r="M11" s="11"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.45">
@@ -3620,10 +4728,19 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
+      <c r="I12" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="J12" t="s">
+        <v>163</v>
+      </c>
+      <c r="K12" t="s">
+        <v>167</v>
+      </c>
+      <c r="L12" s="12">
+        <f>SUMIF(I:I,"Functionality",F:F)</f>
+        <v>0</v>
+      </c>
       <c r="M12" s="12"/>
       <c r="N12" s="12"/>
       <c r="O12" s="12"/>
@@ -3655,6 +4772,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="I13" s="40" t="s">
+        <v>165</v>
+      </c>
+      <c r="J13" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.45">
       <c r="C14" t="s">
@@ -3677,6 +4800,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="I14" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
@@ -3702,6 +4828,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="I15" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="J15" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.45">
       <c r="C16" t="s">
@@ -3724,8 +4856,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="I16" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="J16" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.45">
       <c r="C17" t="s">
         <v>97</v>
       </c>
@@ -3746,8 +4884,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="I17" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="J17" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.45">
       <c r="C18" t="s">
         <v>98</v>
       </c>
@@ -3768,8 +4912,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="I18" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="J18" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.45">
       <c r="C19" t="s">
         <v>99</v>
       </c>
@@ -3790,8 +4940,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="I19" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="J19" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.45">
       <c r="C20" t="s">
         <v>94</v>
       </c>
@@ -3812,8 +4968,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="I20" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
         <v>84</v>
       </c>
@@ -3837,8 +4996,14 @@
         <f t="shared" si="1"/>
         <v>-1750.26</v>
       </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="I21" t="s">
+        <v>161</v>
+      </c>
+      <c r="J21" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
         <v>85</v>
       </c>
@@ -3862,8 +5027,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="I22" t="s">
+        <v>161</v>
+      </c>
+      <c r="J22" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B23" t="s">
         <v>86</v>
       </c>
@@ -3887,8 +5058,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="I23" t="s">
+        <v>161</v>
+      </c>
+      <c r="J23" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B24" t="s">
         <v>87</v>
       </c>
@@ -3912,8 +5089,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="I24" t="s">
+        <v>161</v>
+      </c>
+      <c r="J24" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.45">
       <c r="C25" t="s">
         <v>130</v>
       </c>
@@ -3934,8 +5117,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="I25" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
         <v>88</v>
       </c>
@@ -3959,8 +5145,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="I26" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="J26" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B27" t="s">
         <v>111</v>
       </c>
@@ -3984,8 +5176,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="I27" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="J27" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.45">
       <c r="C28" t="s">
         <v>113</v>
       </c>
@@ -4006,8 +5204,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="I28" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="J28" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B29" t="s">
         <v>132</v>
       </c>
@@ -4031,8 +5235,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="I29" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="J29" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B30" t="s">
         <v>133</v>
       </c>
@@ -4056,8 +5266,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="I30" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.45">
       <c r="C31" t="s">
         <v>136</v>
       </c>
@@ -4078,8 +5291,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="I31" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.45">
       <c r="C32" t="s">
         <v>135</v>
       </c>
@@ -4100,8 +5316,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="I32" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.45">
       <c r="C33" t="s">
         <v>137</v>
       </c>
@@ -4122,8 +5341,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="I33" s="39" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B34" t="s">
         <v>132</v>
       </c>
@@ -4147,8 +5369,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="I34" t="s">
+        <v>163</v>
+      </c>
+      <c r="J34" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.45">
       <c r="C35" t="s">
         <v>146</v>
       </c>
@@ -4169,8 +5397,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="I35" s="39" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B36" t="s">
         <v>145</v>
       </c>
@@ -4194,8 +5425,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="I36" s="12" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B37" t="s">
         <v>151</v>
       </c>
@@ -4219,8 +5453,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="I37" s="12" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B38" t="s">
         <v>153</v>
       </c>
@@ -4244,8 +5481,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="I38" s="12" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B39" t="s">
         <v>155</v>
       </c>
@@ -4269,8 +5509,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="I39" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B40" t="s">
         <v>157</v>
       </c>
@@ -4290,21 +5533,58 @@
       <c r="G40">
         <v>0</v>
       </c>
-      <c r="H40" s="12"/>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="H40" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I40" s="39" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B41" t="s">
+        <v>159</v>
+      </c>
       <c r="C41" t="s">
+        <v>158</v>
+      </c>
+      <c r="D41" s="39">
+        <v>-95</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I41" s="39" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="C42" t="s">
         <v>74</v>
       </c>
-      <c r="D41" s="12"/>
-      <c r="F41" s="12">
-        <f>SUM(F9:F40)</f>
+      <c r="D42" s="12"/>
+      <c r="F42" s="12">
+        <f>SUM(F9:F41)</f>
         <v>-5787.22</v>
       </c>
-      <c r="H41" s="12">
+      <c r="H42" s="12">
         <f>SUM(H9:H39)</f>
         <v>-1750.26</v>
       </c>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="C45" s="12"/>
     </row>
   </sheetData>
   <scenarios current="0" show="0">

</xml_diff>

<commit_message>
updated purchased and alignemnt options
</commit_message>
<xml_diff>
--- a/myrepo/Tesla_Model_3_Loan_Analysis.xlsx
+++ b/myrepo/Tesla_Model_3_Loan_Analysis.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrw7f\github-mwyatt9214\myrepo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mateo\github-mwyatt9214\myrepo\myrepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65942849-CDEC-4263-A2D8-E68B6635E75B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Analysis" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="Insurance" sheetId="5" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -28,14 +27,14 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
     <author>Matt Wyatt</author>
     <author>Matthew Wyatt</author>
   </authors>
   <commentList>
-    <comment ref="Q8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="Q8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -61,7 +60,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="D9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -75,7 +74,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T9" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+    <comment ref="T9" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -99,7 +98,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
+    <comment ref="D10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -113,7 +112,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
+    <comment ref="O10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -127,7 +126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
+    <comment ref="P10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -141,7 +140,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
+    <comment ref="D11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -167,7 +166,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
+    <comment ref="D12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -193,7 +192,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
+    <comment ref="C14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -219,7 +218,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000A000000}">
+    <comment ref="D21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -233,7 +232,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="D22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000B000000}">
+    <comment ref="C22" authorId="2" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Matthew Wyatt:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+https://www.tirerack.com/tires/tires.jsp?tireMake=Michelin&amp;tireModel=Pilot+Sport+4S&amp;frontTire=335YR0PS4SXL&amp;rearTire=73YR0PS4SXL&amp;vehicleSearch=true&amp;fromCompare1=yes&amp;autoMake=Tesla&amp;autoYear=2018&amp;autoModel=Model%203%20With%20Staggered%20Tires&amp;autoModClar=</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -247,7 +270,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000C000000}">
+    <comment ref="D23" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -261,7 +284,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000D000000}">
+    <comment ref="B25" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -287,7 +310,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C28" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000E000000}">
+    <comment ref="C29" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -311,7 +334,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C29" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000F000000}">
+    <comment ref="C30" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -335,7 +358,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C34" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0100-000010000000}">
+    <comment ref="C35" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -349,7 +372,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C35" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0100-000011000000}">
+    <comment ref="C36" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -373,7 +396,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C36" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0100-000012000000}">
+    <comment ref="C37" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -397,7 +420,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="C38" authorId="2" shapeId="0" xr:uid="{28751B4B-0235-4BA5-948B-EE86A4D424BD}">
+    <comment ref="C38" authorId="2" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Matthew Wyatt:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+https://getjeda.com/product/jeda-wireless-pad/</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C39" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -421,7 +468,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C40" authorId="2" shapeId="0" xr:uid="{45812E76-2414-49A4-9A43-2E509EB54DC6}">
+    <comment ref="C41" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -445,12 +492,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="C43" authorId="2" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Matthew Wyatt:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+https://www.reverselogic.us/tesla</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="183">
   <si>
     <t>Total OutOfPocket</t>
   </si>
@@ -755,9 +826,6 @@
     <t>turbine wheels</t>
   </si>
   <si>
-    <t>Pirelli P0 tires</t>
-  </si>
-  <si>
     <t>Springs</t>
   </si>
   <si>
@@ -809,21 +877,9 @@
     <t>15 prop damage</t>
   </si>
   <si>
-    <t>500 ded Comp</t>
-  </si>
-  <si>
-    <t>500 ded Collision</t>
-  </si>
-  <si>
     <t>15/30 uninsured motorist</t>
   </si>
   <si>
-    <t>1500 rantal</t>
-  </si>
-  <si>
-    <t>250 ded mech breakdown</t>
-  </si>
-  <si>
     <t>AAA</t>
   </si>
   <si>
@@ -836,9 +892,6 @@
     <t>1000 ded Collision</t>
   </si>
   <si>
-    <t>Delta/month</t>
-  </si>
-  <si>
     <t>Insurance Differential/Year</t>
   </si>
   <si>
@@ -875,9 +928,6 @@
     <t>Cost</t>
   </si>
   <si>
-    <t>Spent</t>
-  </si>
-  <si>
     <t>Fees</t>
   </si>
   <si>
@@ -905,9 +955,6 @@
     <t>wireless charging pad</t>
   </si>
   <si>
-    <t>nomad</t>
-  </si>
-  <si>
     <t>card rail for key</t>
   </si>
   <si>
@@ -954,12 +1001,81 @@
   </si>
   <si>
     <t>Functionality</t>
+  </si>
+  <si>
+    <t>Credit</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>Brake Pads</t>
+  </si>
+  <si>
+    <t>code:undecided</t>
+  </si>
+  <si>
+    <t>reverse logic</t>
+  </si>
+  <si>
+    <t>jack pads</t>
+  </si>
+  <si>
+    <t>Delta/year</t>
+  </si>
+  <si>
+    <t>just model 3</t>
+  </si>
+  <si>
+    <t>model +mazda</t>
+  </si>
+  <si>
+    <t>132/month</t>
+  </si>
+  <si>
+    <t>165/month</t>
+  </si>
+  <si>
+    <t>jeta</t>
+  </si>
+  <si>
+    <t>Michelin pilot sport 4s</t>
+  </si>
+  <si>
+    <t>handwash stuff</t>
+  </si>
+  <si>
+    <t>elite finish</t>
+  </si>
+  <si>
+    <t>wheels and tires</t>
+  </si>
+  <si>
+    <t>alignment and camber adjustment</t>
+  </si>
+  <si>
+    <t>normal alignment</t>
+  </si>
+  <si>
+    <t>custom alignment</t>
+  </si>
+  <si>
+    <t>alignment</t>
+  </si>
+  <si>
+    <t>Funtionality</t>
+  </si>
+  <si>
+    <t>Speed Element Tuning</t>
+  </si>
+  <si>
+    <t>Wheel Mount and Balance</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="\$#,##0.00_);[Red]&quot;($&quot;#,##0.00\)"/>
@@ -1232,7 +1348,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1276,6 +1392,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1420,8 +1537,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1441,7 +1559,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Features!$K$8:$K$12</c:f>
+              <c:f>Features!$L$8:$L$12</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1464,21 +1582,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Features!$L$8:$L$12</c:f>
+              <c:f>Features!$M$8:$M$12</c:f>
               <c:numCache>
                 <c:formatCode>\$#,##0.00_);[Red]"($"#,##0.00\)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-3387.2200000000003</c:v>
+                  <c:v>-3739.6800000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-550</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-850</c:v>
+                  <c:v>-1312</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1486,7 +1604,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-6671-4A64-8329-11A20DD679EE}"/>
             </c:ext>
@@ -1502,12 +1620,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="625883384"/>
-        <c:axId val="625881088"/>
+        <c:axId val="452171328"/>
+        <c:axId val="448920408"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="625883384"/>
+        <c:axId val="452171328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1544,7 +1662,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="625881088"/>
+        <c:crossAx val="448920408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1552,7 +1670,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="625881088"/>
+        <c:axId val="448920408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1603,7 +1721,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="625883384"/>
+        <c:crossAx val="452171328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1617,14 +1735,14 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2237,8 +2355,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>512044</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>726356</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>1961</xdr:rowOff>
     </xdr:to>
@@ -2247,7 +2365,7 @@
         <xdr:cNvPr id="2" name="CustomShape 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2294,8 +2412,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>512044</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>726356</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>1961</xdr:rowOff>
     </xdr:to>
@@ -2304,7 +2422,7 @@
         <xdr:cNvPr id="3" name="CustomShape 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2351,8 +2469,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>512044</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>726356</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>1961</xdr:rowOff>
     </xdr:to>
@@ -2361,7 +2479,7 @@
         <xdr:cNvPr id="4" name="CustomShape 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2408,8 +2526,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>512044</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>726356</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>1961</xdr:rowOff>
     </xdr:to>
@@ -2418,7 +2536,7 @@
         <xdr:cNvPr id="5" name="CustomShape 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2465,8 +2583,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>512044</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>726356</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>1961</xdr:rowOff>
     </xdr:to>
@@ -2475,7 +2593,7 @@
         <xdr:cNvPr id="6" name="CustomShape 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2522,8 +2640,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>512044</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>726356</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>1961</xdr:rowOff>
     </xdr:to>
@@ -2532,7 +2650,7 @@
         <xdr:cNvPr id="7" name="CustomShape 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2579,8 +2697,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>512044</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>726356</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>1961</xdr:rowOff>
     </xdr:to>
@@ -2589,7 +2707,7 @@
         <xdr:cNvPr id="8" name="CustomShape 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2636,8 +2754,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>512044</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>726356</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>1961</xdr:rowOff>
     </xdr:to>
@@ -2646,7 +2764,7 @@
         <xdr:cNvPr id="9" name="CustomShape 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2695,7 +2813,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2703,7 +2821,7 @@
         <xdr:cNvPr id="1042" name="shapetype_202" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000012040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000012040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2744,7 +2862,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2752,7 +2870,7 @@
         <xdr:cNvPr id="1040" name="shapetype_202" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000010040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000010040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2793,7 +2911,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2801,7 +2919,7 @@
         <xdr:cNvPr id="1038" name="shapetype_202" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000E040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000E040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2842,7 +2960,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2850,7 +2968,7 @@
         <xdr:cNvPr id="1036" name="shapetype_202" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000C040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000C040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2891,7 +3009,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2899,7 +3017,7 @@
         <xdr:cNvPr id="1034" name="shapetype_202" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000A040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2940,7 +3058,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2948,7 +3066,7 @@
         <xdr:cNvPr id="1032" name="shapetype_202" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000008040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2989,7 +3107,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2997,7 +3115,7 @@
         <xdr:cNvPr id="1030" name="shapetype_202" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000006040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3038,7 +3156,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3046,7 +3164,7 @@
         <xdr:cNvPr id="1028" name="shapetype_202" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000004040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3087,7 +3205,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3095,7 +3213,7 @@
         <xdr:cNvPr id="1026" name="shapetype_202" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3128,15 +3246,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>5950</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>72033</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>506013</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>136327</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3144,7 +3262,7 @@
         <xdr:cNvPr id="10" name="Chart 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D52A36F2-0B21-44D2-92A4-2994C2403359}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D52A36F2-0B21-44D2-92A4-2994C2403359}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3427,40 +3545,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q46"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.59765625"/>
-    <col min="3" max="3" width="11.59765625"/>
-    <col min="4" max="4" width="27.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.59765625"/>
-    <col min="6" max="6" width="11.265625"/>
-    <col min="7" max="7" width="25.3984375"/>
-    <col min="8" max="8" width="12.1328125"/>
-    <col min="9" max="9" width="8.59765625"/>
-    <col min="10" max="10" width="17.1328125"/>
+    <col min="1" max="1" width="44.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125"/>
+    <col min="3" max="3" width="11.5703125"/>
+    <col min="4" max="4" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125"/>
+    <col min="6" max="6" width="11.28515625"/>
+    <col min="7" max="7" width="25.42578125"/>
+    <col min="8" max="8" width="12.140625"/>
+    <col min="9" max="9" width="8.5703125"/>
+    <col min="10" max="10" width="17.140625"/>
     <col min="11" max="11" width="28"/>
-    <col min="12" max="12" width="23.73046875"/>
-    <col min="13" max="13" width="9.73046875"/>
-    <col min="14" max="14" width="21.86328125"/>
-    <col min="15" max="15" width="12.59765625"/>
-    <col min="16" max="1025" width="8.59765625"/>
+    <col min="12" max="12" width="23.7109375"/>
+    <col min="13" max="13" width="9.7109375"/>
+    <col min="14" max="14" width="21.85546875"/>
+    <col min="15" max="15" width="12.5703125"/>
+    <col min="16" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="2">
         <f>B5+SUM(B13:B16)</f>
-        <v>-31350.22</v>
+        <v>-30639.68</v>
       </c>
       <c r="G1" s="25" t="s">
         <v>1</v>
@@ -3490,7 +3608,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -3539,7 +3657,7 @@
         <v>600.82026666666673</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -3548,7 +3666,7 @@
         <v>-2397.4299999999998</v>
       </c>
       <c r="D3" s="41" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="E3" s="9">
         <f>E2/B8</f>
@@ -3580,7 +3698,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -3588,7 +3706,7 @@
         <v>-1122</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="E4" s="9">
         <f>B32-E3</f>
@@ -3619,7 +3737,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -3646,7 +3764,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -3680,13 +3798,13 @@
         <v>13750</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B7" s="7">
-        <f>Insurance!D10</f>
-        <v>-786</v>
+        <f>Insurance!D3</f>
+        <v>-337.79999999999995</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>30</v>
@@ -3710,7 +3828,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -3722,21 +3840,21 @@
       </c>
       <c r="E8" s="9">
         <f>E7+B9+B10+B11+((B7/12)*B8)</f>
-        <v>26900.579999999998</v>
+        <v>29589.78</v>
       </c>
       <c r="G8" s="32" t="s">
         <v>46</v>
       </c>
       <c r="H8" s="34">
         <f>H7+E1</f>
-        <v>34656.86</v>
+        <v>35367.4</v>
       </c>
       <c r="M8">
         <f>SUM(M6:M7)</f>
         <v>16350</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -3755,10 +3873,10 @@
       </c>
       <c r="H9" s="35">
         <f>H8-15000</f>
-        <v>19656.86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
+        <v>20367.400000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -3766,7 +3884,7 @@
         <v>7500</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="E10" s="9">
         <v>-753</v>
@@ -3776,10 +3894,10 @@
       </c>
       <c r="H10" s="37">
         <f>H9</f>
-        <v>19656.86</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
+        <v>20367.400000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -3791,26 +3909,26 @@
       </c>
       <c r="E11" s="9">
         <f>B6+E9+E5+B13+B14+B16+E10+B12</f>
-        <v>-79382.46743297427</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
+        <v>-78671.927432974277</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B12" s="7">
         <v>3500</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E12" s="9">
         <f>E11+E8</f>
-        <v>-52481.887432974268</v>
+        <v>-49082.147432974278</v>
       </c>
       <c r="G12" s="42"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -3818,7 +3936,7 @@
         <v>3437</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -3826,7 +3944,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -3834,31 +3952,31 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="11" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:17" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>54</v>
       </c>
       <c r="B16" s="12">
-        <f>Features!F42</f>
-        <v>-5787.22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" s="15" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+        <f>Features!F49</f>
+        <v>-5076.68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
         <v>55</v>
       </c>
       <c r="B17" s="14">
         <f>(E6+E8)/B8</f>
-        <v>-293.49538101353153</v>
+        <v>-256.14538101353151</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B18" s="5">
         <f>B17</f>
-        <v>-293.49538101353153</v>
+        <v>-256.14538101353151</v>
       </c>
       <c r="C18" s="16">
         <v>12</v>
@@ -3882,7 +4000,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -3912,7 +4030,7 @@
         <v>293.2858333333333</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B20" s="10">
         <v>-50000</v>
       </c>
@@ -3941,7 +4059,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B21" s="10">
         <v>-60000</v>
       </c>
@@ -3972,7 +4090,7 @@
         <v>472.87614243637466</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" s="10">
         <v>-70000</v>
       </c>
@@ -3995,7 +4113,7 @@
         <v>-302.10097222222203</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="18">
         <v>-80000</v>
       </c>
@@ -4018,7 +4136,7 @@
         <v>-478.191944444444</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>59</v>
       </c>
@@ -4045,7 +4163,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>60</v>
       </c>
@@ -4071,7 +4189,7 @@
         <v>-114.46875</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B26" s="23">
         <v>3.5000000000000003E-2</v>
       </c>
@@ -4094,7 +4212,7 @@
         <v>-133.546875</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B27" s="23">
         <v>0.04</v>
       </c>
@@ -4117,7 +4235,7 @@
         <v>-152.625</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B28" s="23">
         <v>4.4999999999999998E-2</v>
       </c>
@@ -4140,7 +4258,7 @@
         <v>-171.703125</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B29" s="23">
         <v>0.05</v>
       </c>
@@ -4163,7 +4281,7 @@
         <v>-190.78125</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B30" s="23">
         <v>5.5E-2</v>
       </c>
@@ -4186,7 +4304,7 @@
         <v>-209.859375</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="23">
         <v>0.06</v>
       </c>
@@ -4209,9 +4327,9 @@
         <v>-228.9375</v>
       </c>
     </row>
-    <row r="32" spans="1:11" s="15" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:11" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="13" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B32" s="14">
         <f>-1*PMT(B2/12,B8,E2)</f>
@@ -4221,7 +4339,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B33" s="5">
         <f>B32</f>
         <v>-667.11454768019814</v>
@@ -4245,7 +4363,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -4271,7 +4389,7 @@
         <v>-212.947222222222</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B35" s="10">
         <v>-50000</v>
       </c>
@@ -4294,7 +4412,7 @@
         <v>-389.038194444444</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B36" s="10">
         <v>-60000</v>
       </c>
@@ -4317,7 +4435,7 @@
         <v>-565.12916666666695</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B37" s="10">
         <v>-70000</v>
       </c>
@@ -4340,7 +4458,7 @@
         <v>-741.22013888888898</v>
       </c>
     </row>
-    <row r="38" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="18">
         <v>-80000</v>
       </c>
@@ -4363,7 +4481,7 @@
         <v>-917.31111111111102</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>61</v>
       </c>
@@ -4372,7 +4490,7 @@
         <v>600.82026666666673</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>62</v>
       </c>
@@ -4380,13 +4498,35 @@
         <v>5.95</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>63</v>
       </c>
       <c r="B41">
         <f>(B40/1000)*(1000/453.592)*B39</f>
         <v>7.8812690406062442</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <v>53000</v>
+      </c>
+      <c r="G44">
+        <v>70000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <v>32000</v>
+      </c>
+      <c r="G45">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G46">
+        <f>(G44*F44)+(G45*F45)</f>
+        <v>6910000000</v>
       </c>
     </row>
   </sheetData>
@@ -4396,45 +4536,45 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:U45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:F49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.73046875"/>
-    <col min="5" max="5" width="16.3984375"/>
-    <col min="6" max="6" width="17.59765625"/>
-    <col min="7" max="7" width="18.1328125"/>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375"/>
+    <col min="5" max="5" width="16.42578125"/>
+    <col min="6" max="6" width="17.5703125"/>
+    <col min="7" max="7" width="18.140625"/>
     <col min="8" max="8" width="13"/>
     <col min="9" max="9" width="23"/>
-    <col min="10" max="10" width="22.1328125"/>
-    <col min="11" max="11" width="24.1328125"/>
-    <col min="12" max="12" width="32.86328125"/>
-    <col min="13" max="13" width="13.1328125"/>
-    <col min="14" max="14" width="16.3984375"/>
-    <col min="15" max="15" width="15.1328125"/>
-    <col min="16" max="16" width="25.1328125"/>
+    <col min="10" max="10" width="22.140625"/>
+    <col min="11" max="11" width="24.140625"/>
+    <col min="12" max="12" width="32.85546875"/>
+    <col min="13" max="13" width="13.140625"/>
+    <col min="14" max="14" width="16.42578125"/>
+    <col min="15" max="15" width="15.140625"/>
+    <col min="16" max="16" width="25.140625"/>
     <col min="17" max="17" width="16"/>
-    <col min="18" max="18" width="14.86328125"/>
-    <col min="19" max="19" width="15.265625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="22" max="1025" width="8.59765625"/>
+    <col min="18" max="18" width="14.85546875"/>
+    <col min="19" max="19" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -4466,7 +4606,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>-35000</v>
       </c>
@@ -4495,7 +4635,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -4524,7 +4664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ref="A5:I5" si="0">IF(A4=1,A3,0)</f>
         <v>-35000</v>
@@ -4566,7 +4706,7 @@
         <v>-44000</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>80</v>
       </c>
@@ -4576,29 +4716,32 @@
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
       <c r="F8" s="12" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="G8" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="H8" t="s">
-        <v>141</v>
+        <v>160</v>
       </c>
       <c r="I8" s="39" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="J8" s="39" t="s">
-        <v>162</v>
-      </c>
-      <c r="K8" t="s">
-        <v>161</v>
-      </c>
-      <c r="L8" s="12">
-        <f>SUMIF(I:I,"Performance",F:F)</f>
-        <v>-3387.2200000000003</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
+        <v>152</v>
+      </c>
+      <c r="K8" s="39" t="s">
+        <v>154</v>
+      </c>
+      <c r="L8" t="s">
+        <v>153</v>
+      </c>
+      <c r="M8" s="12">
+        <f>SUMIF(J:J,"Performance",F:F)</f>
+        <v>-3739.6800000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>82</v>
       </c>
@@ -4612,7 +4755,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="12">
-        <f t="shared" ref="F9:H41" si="1">IF(E9=1,D9,0)</f>
+        <f t="shared" ref="F9:H43" si="1">IF(E9=1,D9,0)</f>
         <v>0</v>
       </c>
       <c r="G9">
@@ -4622,21 +4765,25 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I9" t="s">
-        <v>161</v>
+      <c r="I9" s="12">
+        <f>IF(G9=2,F9,0)</f>
+        <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="K9" t="s">
-        <v>163</v>
-      </c>
-      <c r="L9" s="12">
-        <f>SUMIF(I:I,"Aesthetic",F:F)</f>
-        <v>-1000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.45">
+        <v>155</v>
+      </c>
+      <c r="L9" t="s">
+        <v>155</v>
+      </c>
+      <c r="M9" s="12">
+        <f>SUMIF(J:J,"Aesthetic",F:F)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10" t="s">
@@ -4659,21 +4806,25 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I10" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="J10" t="s">
-        <v>163</v>
+      <c r="I10" s="12">
+        <f t="shared" ref="I10:I43" si="2">IF(G10=2,F10,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>153</v>
       </c>
       <c r="K10" t="s">
-        <v>164</v>
-      </c>
-      <c r="L10" s="12">
-        <f>SUMIF(I:I,"Comfort",F:F)</f>
-        <v>-550</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
+        <v>155</v>
+      </c>
+      <c r="L10" t="s">
+        <v>156</v>
+      </c>
+      <c r="M10" s="12">
+        <f>SUMIF(J:J,"Comfort",F:F)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>91</v>
       </c>
@@ -4694,20 +4845,23 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I11" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="J11" s="11"/>
-      <c r="K11" t="s">
-        <v>165</v>
-      </c>
-      <c r="L11" s="12">
-        <f>SUMIF(I:I,"Maintenance",F:F)</f>
-        <v>-850</v>
-      </c>
-      <c r="M11" s="11"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="I11" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="K11" s="11"/>
+      <c r="L11" t="s">
+        <v>157</v>
+      </c>
+      <c r="M11" s="12">
+        <f>SUMIF(J:J,"Maintenance",F:F)</f>
+        <v>-1312</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>92</v>
       </c>
@@ -4728,20 +4882,23 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I12" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="J12" t="s">
-        <v>163</v>
+      <c r="I12" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>156</v>
       </c>
       <c r="K12" t="s">
-        <v>167</v>
-      </c>
-      <c r="L12" s="12">
-        <f>SUMIF(I:I,"Functionality",F:F)</f>
-        <v>0</v>
-      </c>
-      <c r="M12" s="12"/>
+        <v>155</v>
+      </c>
+      <c r="L12" t="s">
+        <v>159</v>
+      </c>
+      <c r="M12" s="12">
+        <f>SUMIF(J:J,"Functionality",F:F)</f>
+        <v>0</v>
+      </c>
       <c r="N12" s="12"/>
       <c r="O12" s="12"/>
       <c r="P12" s="12"/>
@@ -4751,7 +4908,7 @@
       <c r="T12" s="12"/>
       <c r="U12" s="12"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>93</v>
       </c>
@@ -4772,14 +4929,18 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I13" s="40" t="s">
-        <v>165</v>
-      </c>
-      <c r="J13" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="I13" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="40" t="s">
+        <v>157</v>
+      </c>
+      <c r="K13" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>94</v>
       </c>
@@ -4800,11 +4961,15 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I14" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="I14" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>83</v>
       </c>
@@ -4828,14 +4993,18 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I15" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="J15" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="I15" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="K15" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>96</v>
       </c>
@@ -4856,14 +5025,18 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I16" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="J16" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="I16" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="K16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>97</v>
       </c>
@@ -4884,14 +5057,18 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I17" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="J17" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="I17" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="K17" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>98</v>
       </c>
@@ -4912,14 +5089,18 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I18" s="39" t="s">
-        <v>165</v>
-      </c>
-      <c r="J18" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="I18" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="K18" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>99</v>
       </c>
@@ -4940,14 +5121,18 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I19" s="39" t="s">
-        <v>165</v>
-      </c>
-      <c r="J19" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="I19" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="K19" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>94</v>
       </c>
@@ -4955,11 +5140,11 @@
         <v>-1000</v>
       </c>
       <c r="E20" s="40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" s="12">
         <f t="shared" si="1"/>
-        <v>-1000</v>
+        <v>0</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -4968,11 +5153,15 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I20" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="I20" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J20" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>84</v>
       </c>
@@ -4996,595 +5185,928 @@
         <f t="shared" si="1"/>
         <v>-1750.26</v>
       </c>
-      <c r="I21" t="s">
-        <v>161</v>
+      <c r="I21" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="J21" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.45">
+        <v>153</v>
+      </c>
+      <c r="K21" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>85</v>
       </c>
       <c r="C22" t="s">
-        <v>101</v>
+        <v>172</v>
       </c>
       <c r="D22" s="12">
-        <v>-971.96</v>
+        <v>-1233.06</v>
       </c>
       <c r="E22" s="11">
         <v>1</v>
       </c>
       <c r="F22" s="12">
-        <f t="shared" si="1"/>
-        <v>-971.96</v>
+        <v>-1297.96</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I22" t="s">
-        <v>161</v>
+        <v>-1297.96</v>
+      </c>
+      <c r="I22" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="J22" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.45">
+        <v>153</v>
+      </c>
+      <c r="K22" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>86</v>
       </c>
       <c r="C23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D23" s="12">
-        <v>-665</v>
+        <v>-691.46</v>
       </c>
       <c r="E23" s="11">
         <v>1</v>
       </c>
       <c r="F23" s="12">
         <f t="shared" si="1"/>
-        <v>-665</v>
+        <v>-691.46</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I23" t="s">
-        <v>161</v>
+        <v>-691.46</v>
+      </c>
+      <c r="I23" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="J23" t="s">
+        <v>153</v>
+      </c>
+      <c r="K23" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>162</v>
+      </c>
+      <c r="D24" s="12">
+        <v>-350</v>
+      </c>
+      <c r="E24" s="40">
+        <v>0</v>
+      </c>
+      <c r="F24" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J24" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" t="s">
+        <v>102</v>
+      </c>
+      <c r="D25" s="12">
+        <v>-1380</v>
+      </c>
+      <c r="E25" s="11">
+        <v>0</v>
+      </c>
+      <c r="F25" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I25" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J25" t="s">
+        <v>153</v>
+      </c>
+      <c r="K25" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>124</v>
+      </c>
+      <c r="D26" s="12">
+        <v>-427.66</v>
+      </c>
+      <c r="E26" s="11">
+        <v>0</v>
+      </c>
+      <c r="F26" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I26" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J26" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>88</v>
+      </c>
+      <c r="C27" t="s">
+        <v>103</v>
+      </c>
+      <c r="D27" s="12">
+        <v>-850</v>
+      </c>
+      <c r="E27" s="11">
+        <v>1</v>
+      </c>
+      <c r="F27" s="12">
+        <f t="shared" si="1"/>
+        <v>-850</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I27" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J27" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="K27" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>110</v>
+      </c>
+      <c r="C28" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" s="12">
+        <v>-1700</v>
+      </c>
+      <c r="E28" s="11">
+        <v>0</v>
+      </c>
+      <c r="F28" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I28" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J28" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="K28" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>112</v>
+      </c>
+      <c r="D29" s="12">
+        <v>-550</v>
+      </c>
+      <c r="E29" s="11">
+        <v>0</v>
+      </c>
+      <c r="F29" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I29" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J29" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="K29" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>126</v>
+      </c>
+      <c r="C30" t="s">
+        <v>125</v>
+      </c>
+      <c r="D30" s="12">
+        <v>-30</v>
+      </c>
+      <c r="E30" s="11">
+        <v>1</v>
+      </c>
+      <c r="F30" s="12">
+        <f t="shared" si="1"/>
+        <v>-30</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30" s="12">
+        <f t="shared" si="1"/>
+        <v>-30</v>
+      </c>
+      <c r="I30" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J30" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="K30" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B24" t="s">
-        <v>87</v>
-      </c>
-      <c r="C24" t="s">
-        <v>103</v>
-      </c>
-      <c r="D24" s="12">
-        <v>-1380</v>
-      </c>
-      <c r="E24" s="11">
-        <v>0</v>
-      </c>
-      <c r="F24" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I24" t="s">
-        <v>161</v>
-      </c>
-      <c r="J24" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="C25" t="s">
+      <c r="B31" t="s">
+        <v>127</v>
+      </c>
+      <c r="C31" t="s">
+        <v>128</v>
+      </c>
+      <c r="D31" s="12">
+        <v>-100</v>
+      </c>
+      <c r="E31" s="11">
+        <v>0</v>
+      </c>
+      <c r="F31" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I31" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J31" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
         <v>130</v>
       </c>
-      <c r="D25" s="12">
-        <v>-427.66</v>
-      </c>
-      <c r="E25" s="11">
-        <v>0</v>
-      </c>
-      <c r="F25" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
-      <c r="H25" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I25" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B26" t="s">
-        <v>88</v>
-      </c>
-      <c r="C26" t="s">
-        <v>104</v>
-      </c>
-      <c r="D26" s="12">
-        <v>-850</v>
-      </c>
-      <c r="E26" s="11">
+      <c r="D32" s="12">
+        <v>-16</v>
+      </c>
+      <c r="E32" s="11">
+        <v>0</v>
+      </c>
+      <c r="F32" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I32" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J32" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>129</v>
+      </c>
+      <c r="D33" s="12">
+        <v>-12</v>
+      </c>
+      <c r="E33" s="11">
+        <v>0</v>
+      </c>
+      <c r="F33" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I33" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J33" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>131</v>
+      </c>
+      <c r="D34" s="12">
+        <v>-46</v>
+      </c>
+      <c r="E34" s="11">
         <v>1</v>
       </c>
-      <c r="F26" s="12">
-        <f t="shared" si="1"/>
-        <v>-850</v>
-      </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="H26" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I26" s="39" t="s">
+      <c r="F34" s="12">
+        <f t="shared" si="1"/>
+        <v>-46</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34" s="12">
+        <f t="shared" si="1"/>
+        <v>-46</v>
+      </c>
+      <c r="I34" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J34" s="39" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>126</v>
+      </c>
+      <c r="C35" t="s">
+        <v>132</v>
+      </c>
+      <c r="D35" s="12">
+        <v>-30</v>
+      </c>
+      <c r="E35" s="11">
+        <v>0</v>
+      </c>
+      <c r="F35" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I35" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J35" t="s">
+        <v>155</v>
+      </c>
+      <c r="K35" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>139</v>
+      </c>
+      <c r="D36" s="12">
+        <v>-18</v>
+      </c>
+      <c r="E36" s="40">
+        <v>0</v>
+      </c>
+      <c r="F36" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I36" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J36" s="39" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>138</v>
+      </c>
+      <c r="C37" t="s">
+        <v>137</v>
+      </c>
+      <c r="D37" s="39">
+        <v>-29</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I37" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J37" s="12" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>171</v>
+      </c>
+      <c r="C38" t="s">
+        <v>143</v>
+      </c>
+      <c r="D38" s="39">
+        <v>-100</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I38" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J38" s="12" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>145</v>
+      </c>
+      <c r="C39" t="s">
+        <v>144</v>
+      </c>
+      <c r="D39" s="39">
+        <v>-15</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I39" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J39" s="12" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>147</v>
+      </c>
+      <c r="C40" t="s">
+        <v>146</v>
+      </c>
+      <c r="D40" s="39">
+        <v>-20</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I40" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J40" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>149</v>
+      </c>
+      <c r="C41" t="s">
+        <v>148</v>
+      </c>
+      <c r="D41" s="39">
+        <v>-440</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I41" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J41" s="39" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>151</v>
+      </c>
+      <c r="C42" t="s">
+        <v>150</v>
+      </c>
+      <c r="D42" s="39">
+        <v>-95</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I42" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J42" s="39" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>164</v>
+      </c>
+      <c r="C43" t="s">
         <v>165</v>
       </c>
-      <c r="J26" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B27" t="s">
-        <v>111</v>
-      </c>
-      <c r="C27" t="s">
-        <v>112</v>
-      </c>
-      <c r="D27" s="12">
-        <v>-1700</v>
-      </c>
-      <c r="E27" s="11">
-        <v>0</v>
-      </c>
-      <c r="F27" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-      <c r="H27" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I27" s="39" t="s">
-        <v>165</v>
-      </c>
-      <c r="J27" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="C28" t="s">
-        <v>113</v>
-      </c>
-      <c r="D28" s="12">
-        <v>-550</v>
-      </c>
-      <c r="E28" s="11">
+      <c r="D43" s="39">
+        <v>-25</v>
+      </c>
+      <c r="E43">
         <v>1</v>
       </c>
-      <c r="F28" s="12">
-        <f t="shared" si="1"/>
-        <v>-550</v>
-      </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
-      <c r="H28" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I28" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="J28" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B29" t="s">
-        <v>132</v>
-      </c>
-      <c r="C29" t="s">
-        <v>131</v>
-      </c>
-      <c r="D29" s="12">
-        <v>-30</v>
-      </c>
-      <c r="E29" s="11">
-        <v>0</v>
-      </c>
-      <c r="F29" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
-      <c r="H29" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I29" s="39" t="s">
-        <v>165</v>
-      </c>
-      <c r="J29" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B30" t="s">
-        <v>133</v>
-      </c>
-      <c r="C30" t="s">
-        <v>134</v>
-      </c>
-      <c r="D30" s="12">
+      <c r="F43" s="12">
+        <f t="shared" si="1"/>
+        <v>-25</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="H43" s="12">
+        <f t="shared" si="1"/>
+        <v>-25</v>
+      </c>
+      <c r="I43" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J43" s="39" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>174</v>
+      </c>
+      <c r="C44" t="s">
+        <v>173</v>
+      </c>
+      <c r="D44" s="39"/>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44" s="12">
+        <f t="shared" ref="F44" si="3">IF(E44=1,D44,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44" s="12">
+        <f t="shared" ref="H44" si="4">IF(G44=1,F44,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I44" s="12">
+        <f t="shared" ref="I44" si="5">IF(G44=2,F44,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J44" s="39" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>178</v>
+      </c>
+      <c r="C45" t="s">
+        <v>179</v>
+      </c>
+      <c r="D45" s="39">
+        <v>-330</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45" s="12">
+        <f t="shared" ref="F45" si="6">IF(E45=1,D45,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45" s="12">
+        <f t="shared" ref="H45" si="7">IF(G45=1,F45,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I45" s="12">
+        <f t="shared" ref="I45" si="8">IF(G45=2,F45,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J45" s="39" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>175</v>
+      </c>
+      <c r="D46" s="39">
+        <v>-186</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46" s="12">
+        <f t="shared" ref="F46:F48" si="9">IF(E46=1,D46,0)</f>
+        <v>-186</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46" s="12">
+        <f t="shared" ref="H46:H48" si="10">IF(G46=1,F46,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I46" s="12">
+        <f t="shared" ref="I46:I48" si="11">IF(G46=2,F46,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J46" s="39" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>181</v>
+      </c>
+      <c r="C47" t="s">
+        <v>179</v>
+      </c>
+      <c r="D47" s="39">
         <v>-100</v>
       </c>
-      <c r="E30" s="11">
-        <v>0</v>
-      </c>
-      <c r="F30" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-      <c r="H30" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I30" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="C31" t="s">
-        <v>136</v>
-      </c>
-      <c r="D31" s="12">
-        <v>-16</v>
-      </c>
-      <c r="E31" s="11">
-        <v>0</v>
-      </c>
-      <c r="F31" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
-      <c r="H31" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I31" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="C32" t="s">
-        <v>135</v>
-      </c>
-      <c r="D32" s="12">
-        <v>-12</v>
-      </c>
-      <c r="E32" s="11">
-        <v>0</v>
-      </c>
-      <c r="F32" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-      <c r="H32" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I32" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="C33" t="s">
-        <v>137</v>
-      </c>
-      <c r="D33" s="12">
-        <v>-46</v>
-      </c>
-      <c r="E33" s="11">
-        <v>0</v>
-      </c>
-      <c r="F33" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G33">
-        <v>0</v>
-      </c>
-      <c r="H33" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I33" s="39" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B34" t="s">
-        <v>132</v>
-      </c>
-      <c r="C34" t="s">
-        <v>138</v>
-      </c>
-      <c r="D34" s="12">
-        <v>-30</v>
-      </c>
-      <c r="E34" s="11">
-        <v>0</v>
-      </c>
-      <c r="F34" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-      <c r="H34" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I34" t="s">
-        <v>163</v>
-      </c>
-      <c r="J34" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="C35" t="s">
-        <v>146</v>
-      </c>
-      <c r="D35" s="12">
-        <v>-18</v>
-      </c>
-      <c r="E35" s="40">
-        <v>0</v>
-      </c>
-      <c r="F35" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G35">
-        <v>0</v>
-      </c>
-      <c r="H35" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I35" s="39" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B36" t="s">
-        <v>145</v>
-      </c>
-      <c r="C36" t="s">
-        <v>144</v>
-      </c>
-      <c r="D36" s="39">
-        <v>-29</v>
-      </c>
-      <c r="E36">
-        <v>0</v>
-      </c>
-      <c r="F36" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G36">
-        <v>0</v>
-      </c>
-      <c r="H36" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I36" s="12" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B37" t="s">
-        <v>151</v>
-      </c>
-      <c r="C37" t="s">
-        <v>150</v>
-      </c>
-      <c r="D37" s="39">
-        <v>-129</v>
-      </c>
-      <c r="E37">
-        <v>0</v>
-      </c>
-      <c r="F37" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G37">
-        <v>0</v>
-      </c>
-      <c r="H37" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I37" s="12" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B38" t="s">
-        <v>153</v>
-      </c>
-      <c r="C38" t="s">
-        <v>152</v>
-      </c>
-      <c r="D38" s="39">
-        <v>-15</v>
-      </c>
-      <c r="E38">
-        <v>0</v>
-      </c>
-      <c r="F38" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G38">
-        <v>0</v>
-      </c>
-      <c r="H38" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I38" s="12" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B39" t="s">
-        <v>155</v>
-      </c>
-      <c r="C39" t="s">
-        <v>154</v>
-      </c>
-      <c r="D39" s="39">
-        <v>-20</v>
-      </c>
-      <c r="E39">
-        <v>0</v>
-      </c>
-      <c r="F39" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G39">
-        <v>0</v>
-      </c>
-      <c r="H39" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I39" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B40" t="s">
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47" s="12">
+        <f t="shared" si="9"/>
+        <v>-100</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47" s="12">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="I47" s="12">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="J47" s="39" t="s">
         <v>157</v>
       </c>
-      <c r="C40" t="s">
-        <v>156</v>
-      </c>
-      <c r="D40" s="39">
-        <v>-440</v>
-      </c>
-      <c r="E40">
-        <v>0</v>
-      </c>
-      <c r="F40" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G40">
-        <v>0</v>
-      </c>
-      <c r="H40" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I40" s="39" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B41" t="s">
-        <v>159</v>
-      </c>
-      <c r="C41" t="s">
-        <v>158</v>
-      </c>
-      <c r="D41" s="39">
-        <v>-95</v>
-      </c>
-      <c r="E41">
-        <v>0</v>
-      </c>
-      <c r="F41" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G41">
-        <v>0</v>
-      </c>
-      <c r="H41" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I41" s="39" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="C42" t="s">
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>182</v>
+      </c>
+      <c r="D48" s="39">
+        <v>-100</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48" s="12">
+        <f t="shared" si="9"/>
+        <v>-100</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48" s="12">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="I48" s="12">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="J48" s="39" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
         <v>74</v>
       </c>
-      <c r="D42" s="12"/>
-      <c r="F42" s="12">
-        <f>SUM(F9:F41)</f>
-        <v>-5787.22</v>
-      </c>
-      <c r="H42" s="12">
-        <f>SUM(H9:H39)</f>
-        <v>-1750.26</v>
-      </c>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="C45" s="12"/>
+      <c r="D49" s="12"/>
+      <c r="F49" s="12">
+        <f>SUM(F9:F48)</f>
+        <v>-5076.68</v>
+      </c>
+      <c r="H49" s="12">
+        <f>SUM(H9:H40)</f>
+        <v>-3815.6800000000003</v>
+      </c>
+      <c r="I49" s="12">
+        <f>SUM(I9:I40)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>178</v>
+      </c>
+      <c r="B51" t="s">
+        <v>175</v>
+      </c>
+      <c r="C51">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>176</v>
+      </c>
+      <c r="C52" s="12">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>177</v>
+      </c>
+      <c r="C53">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F58">
+        <f>SUM(F56:F57)</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <scenarios current="0" show="0">
@@ -5607,111 +6129,128 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D2">
         <f>-1*93*12</f>
         <v>-1116</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" t="s">
         <v>116</v>
       </c>
-      <c r="B3" t="s">
-        <v>117</v>
-      </c>
       <c r="C3">
-        <v>-1828</v>
+        <v>-1453.8</v>
       </c>
       <c r="D3">
         <f>(C3-D2)</f>
-        <v>-712</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+        <v>-337.79999999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B5" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B6" t="s">
+      <c r="B8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8">
+        <v>-1902</v>
+      </c>
+      <c r="D8">
+        <f>(C8-D2)</f>
+        <v>-786</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B7" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B8" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B9" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>124</v>
-      </c>
-      <c r="B10" t="s">
-        <v>117</v>
-      </c>
-      <c r="C10">
-        <v>-1902</v>
-      </c>
-      <c r="D10">
-        <f>(C10-D2)</f>
-        <v>-786</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B11" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B13" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B14" t="s">
-        <v>121</v>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>168</v>
+      </c>
+      <c r="D14" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <f>900.4*2</f>
+        <v>1800.8</v>
+      </c>
+      <c r="D15">
+        <f>726.9*2</f>
+        <v>1453.8</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>170</v>
+      </c>
+      <c r="D17" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -5720,39 +6259,39 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="60.3984375"/>
-    <col min="2" max="1025" width="8.59765625"/>
+    <col min="1" max="1" width="60.42578125"/>
+    <col min="2" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" t="s">
         <v>105</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>107</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>109</v>
-      </c>
-      <c r="B5" t="s">
-        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated aftermarket and added payment tracking
</commit_message>
<xml_diff>
--- a/myrepo/Tesla_Model_3_Loan_Analysis.xlsx
+++ b/myrepo/Tesla_Model_3_Loan_Analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993"/>
   </bookViews>
   <sheets>
     <sheet name="Analysis" sheetId="1" r:id="rId1"/>
@@ -358,7 +358,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C35" authorId="2" shapeId="0">
+    <comment ref="C36" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -372,7 +372,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C36" authorId="2" shapeId="0">
+    <comment ref="C37" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -396,7 +396,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C37" authorId="2" shapeId="0">
+    <comment ref="C38" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -420,7 +420,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C38" authorId="2" shapeId="0">
+    <comment ref="C39" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -444,7 +444,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C39" authorId="2" shapeId="0">
+    <comment ref="C40" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -468,7 +468,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C41" authorId="2" shapeId="0">
+    <comment ref="C42" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -492,7 +492,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C43" authorId="2" shapeId="0">
+    <comment ref="C44" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -516,12 +516,61 @@
         </r>
       </text>
     </comment>
+    <comment ref="C51" authorId="2" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Matthew Wyatt:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+https://www.amazon.com/dp/B07F27XFB7/ref=as_li_ss_tl?coliid=I1KAMM11G4F458&amp;colid=2AILEG0AAFICG&amp;psc=0&amp;ref_=lv_ov_lig_dp_it&amp;linkCode=sl1&amp;tag=electrek-20&amp;linkId=8e22251f1beb1f6c2c256f7dcb12894e&amp;language=en_US</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C52" authorId="2" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Matthew Wyatt:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+https://www.autoanything.com/floor-mats/3d-maxpider-kagu-floor-mats   
+https://www.amazon.com/gp/product/B07D61H81B/ref=s9_dcacsd_dcoop_bw_c_x_3_w</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="194">
   <si>
     <t>Total OutOfPocket</t>
   </si>
@@ -685,9 +734,6 @@
     <t>KTM Motorcycle</t>
   </si>
   <si>
-    <t>After Market Parts</t>
-  </si>
-  <si>
     <t>Net Cost/Month</t>
   </si>
   <si>
@@ -1036,9 +1082,6 @@
     <t>165/month</t>
   </si>
   <si>
-    <t>jeta</t>
-  </si>
-  <si>
     <t>Michelin pilot sport 4s</t>
   </si>
   <si>
@@ -1070,15 +1113,55 @@
   </si>
   <si>
     <t>Wheel Mount and Balance</t>
+  </si>
+  <si>
+    <t>nomad</t>
+  </si>
+  <si>
+    <t>Door sill clear vinyl</t>
+  </si>
+  <si>
+    <t>floor mats</t>
+  </si>
+  <si>
+    <t>autoanything.com</t>
+  </si>
+  <si>
+    <t>Springs install</t>
+  </si>
+  <si>
+    <t>P3D logo</t>
+  </si>
+  <si>
+    <t>After Market Parts(Want)</t>
+  </si>
+  <si>
+    <t>After Market Parts(Spent)</t>
+  </si>
+  <si>
+    <t>Date of Purchase</t>
+  </si>
+  <si>
+    <t>Current Date</t>
+  </si>
+  <si>
+    <t>Actual Raw Total</t>
+  </si>
+  <si>
+    <t>Current Payed Total Towards Loan</t>
+  </si>
+  <si>
+    <t>Remaining Loan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="\$#,##0.00_);[Red]&quot;($&quot;#,##0.00\)"/>
+    <numFmt numFmtId="168" formatCode="#,##0.0000000000;[Red]#,##0.0000000000"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -1284,7 +1367,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1330,6 +1413,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1587,16 +1672,16 @@
                 <c:formatCode>\$#,##0.00_);[Red]"($"#,##0.00\)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-3739.6800000000003</c:v>
+                  <c:v>-3348.2200000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>-150</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1462</c:v>
+                  <c:v>-1276</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1620,12 +1705,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="458168432"/>
-        <c:axId val="458168824"/>
+        <c:axId val="432012832"/>
+        <c:axId val="432013224"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="458168432"/>
+        <c:axId val="432012832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1662,7 +1747,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="458168824"/>
+        <c:crossAx val="432013224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1670,7 +1755,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="458168824"/>
+        <c:axId val="432013224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1721,7 +1806,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="458168432"/>
+        <c:crossAx val="432012832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2813,7 +2898,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2862,7 +2947,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2911,7 +2996,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2960,7 +3045,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3009,7 +3094,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3058,7 +3143,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3107,7 +3192,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3156,7 +3241,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3205,7 +3290,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3546,10 +3631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q46"/>
+  <dimension ref="A1:Q49"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3557,8 +3642,8 @@
     <col min="1" max="1" width="44.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5703125"/>
     <col min="3" max="3" width="11.5703125"/>
-    <col min="4" max="4" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125"/>
+    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.28515625"/>
     <col min="7" max="7" width="25.42578125"/>
     <col min="8" max="8" width="12.140625"/>
@@ -3578,7 +3663,7 @@
       </c>
       <c r="E1" s="2">
         <f>B5+SUM(B13:B16)</f>
-        <v>-30789.68</v>
+        <v>-30762.22</v>
       </c>
       <c r="G1" s="25" t="s">
         <v>1</v>
@@ -3666,7 +3751,7 @@
         <v>-2397.4299999999998</v>
       </c>
       <c r="D3" s="41" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E3" s="9">
         <f>E2/B8</f>
@@ -3706,10 +3791,10 @@
         <v>-1122</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E4" s="9">
-        <f>B32-E3</f>
+        <f>B35-E3</f>
         <v>-38.9652421246426</v>
       </c>
       <c r="G4" s="29" t="s">
@@ -3800,7 +3885,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B7" s="7">
         <f>Insurance!D3</f>
@@ -3810,8 +3895,8 @@
         <v>30</v>
       </c>
       <c r="E7" s="9">
-        <f>ABS(((B3+B4)/12)*B8)</f>
-        <v>21116.579999999998</v>
+        <f>(ABS(B3+B4)+B7)/12*B8</f>
+        <v>19089.78</v>
       </c>
       <c r="G7" s="32" t="s">
         <v>42</v>
@@ -3839,7 +3924,7 @@
         <v>35</v>
       </c>
       <c r="E8" s="9">
-        <f>E7+B9+B10+B11+((B7/12)*B8)</f>
+        <f>E7+B9+B10+B11</f>
         <v>29589.78</v>
       </c>
       <c r="G8" s="32" t="s">
@@ -3847,7 +3932,7 @@
       </c>
       <c r="H8" s="34">
         <f>H7+E1</f>
-        <v>35217.4</v>
+        <v>35244.86</v>
       </c>
       <c r="M8">
         <f>SUM(M6:M7)</f>
@@ -3873,7 +3958,7 @@
       </c>
       <c r="H9" s="35">
         <f>H8-15000</f>
-        <v>20217.400000000001</v>
+        <v>20244.86</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -3884,7 +3969,7 @@
         <v>7500</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E10" s="9">
         <v>-753</v>
@@ -3894,7 +3979,7 @@
       </c>
       <c r="H10" s="37">
         <f>H9</f>
-        <v>20217.400000000001</v>
+        <v>20244.86</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -3908,23 +3993,23 @@
         <v>45</v>
       </c>
       <c r="E11" s="9">
-        <f>B6+E9+E5+B13+B14+B16+E10+B12</f>
-        <v>-78821.927432974277</v>
+        <f>B6+E9+E5+B16+E10</f>
+        <v>-86731.46743297427</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B12" s="7">
         <v>3500</v>
       </c>
-      <c r="D12" s="24" t="s">
-        <v>113</v>
+      <c r="D12" s="38" t="s">
+        <v>191</v>
       </c>
       <c r="E12" s="9">
-        <f>E11+E8</f>
-        <v>-49232.147432974278</v>
+        <f>-75226.75-B12+B16</f>
+        <v>-83925.97</v>
       </c>
       <c r="G12" s="42"/>
     </row>
@@ -3935,6 +4020,13 @@
       <c r="B13" s="7">
         <v>3437</v>
       </c>
+      <c r="D13" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="E13" s="9">
+        <f>E11+E8</f>
+        <v>-57141.687432974271</v>
+      </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -3943,6 +4035,13 @@
       <c r="B14" s="7">
         <v>1000</v>
       </c>
+      <c r="D14" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="E14" s="9">
+        <f ca="1">((MONTH(B19-B18)-1)*(B35))</f>
+        <v>-667.11454768019814</v>
+      </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -3951,582 +4050,616 @@
       <c r="B15" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D15" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="E15" s="9">
+        <f ca="1">E2-E14</f>
+        <v>-44559.635452319802</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="B16" s="12">
+        <f>Features!F53</f>
+        <v>-5199.22</v>
+      </c>
+      <c r="E16" s="44"/>
+    </row>
+    <row r="17" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="40" t="s">
+        <v>188</v>
+      </c>
+      <c r="B17" s="12">
+        <f>Features!H53</f>
+        <v>-4599.22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="B18" s="43">
+        <v>43374</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="B19" s="43">
+        <f ca="1">TODAY()</f>
+        <v>43423</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="12">
-        <f>Features!F49</f>
-        <v>-5226.68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17" s="14">
+      <c r="B20" s="14">
         <f>(E6+E8)/B8</f>
         <v>-256.14538101353151</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C20" s="15" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="5">
-        <f>B17</f>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="5">
+        <f>B20</f>
         <v>-256.14538101353151</v>
       </c>
-      <c r="C18" s="16">
+      <c r="C21" s="16">
         <v>12</v>
       </c>
-      <c r="D18" s="16">
+      <c r="D21" s="16">
         <v>24</v>
       </c>
-      <c r="E18" s="16">
+      <c r="E21" s="16">
         <v>36</v>
       </c>
-      <c r="F18" s="16">
+      <c r="F21" s="16">
         <v>48</v>
       </c>
-      <c r="G18" s="16">
+      <c r="G21" s="16">
         <v>60</v>
       </c>
-      <c r="H18" s="16">
+      <c r="H21" s="16">
         <v>72</v>
       </c>
-      <c r="J18" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="J21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B22" s="10">
         <v>-40000</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C22" s="10">
         <v>52.560833333333299</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D22" s="10">
         <v>156.72749999999999</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E22" s="10">
         <v>191.44972222222199</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F22" s="10">
         <v>208.81083333333299</v>
       </c>
-      <c r="G19" s="10">
+      <c r="G22" s="10">
         <v>219.22749999999999</v>
       </c>
-      <c r="H19" s="10">
+      <c r="H22" s="10">
         <v>226.17194444444399</v>
       </c>
-      <c r="J19" s="7">
+      <c r="J22" s="7">
         <f>ABS((B3+B4)/12)</f>
         <v>293.2858333333333</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="10">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="10">
         <v>-50000</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C23" s="10">
         <v>-870.05791666666698</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D23" s="10">
         <v>-317.97458333333299</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E23" s="10">
         <v>-133.94680555555601</v>
       </c>
-      <c r="F20" s="10">
+      <c r="F23" s="10">
         <v>-41.932916666666699</v>
       </c>
-      <c r="G20" s="10">
+      <c r="G23" s="10">
         <v>13.275416666666599</v>
       </c>
-      <c r="H20" s="10">
+      <c r="H23" s="10">
         <v>50.080972222222201</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J23" t="s">
+        <v>56</v>
+      </c>
+      <c r="K23" t="s">
         <v>57</v>
       </c>
-      <c r="K20" t="s">
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="10">
+        <v>-60000</v>
+      </c>
+      <c r="C24" s="10">
+        <v>-1792.6766666666699</v>
+      </c>
+      <c r="D24" s="10">
+        <v>-792.67666666666696</v>
+      </c>
+      <c r="E24" s="10">
+        <v>-459.34333333333302</v>
+      </c>
+      <c r="F24" s="10">
+        <v>-292.67666666666702</v>
+      </c>
+      <c r="G24" s="10">
+        <v>-192.67666666666699</v>
+      </c>
+      <c r="H24" s="10">
+        <v>-126.01</v>
+      </c>
+      <c r="J24" s="7">
+        <f>J22*120</f>
+        <v>35194.299999999996</v>
+      </c>
+      <c r="K24">
+        <f>60*B44</f>
+        <v>472.87614243637466</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="10">
+        <v>-70000</v>
+      </c>
+      <c r="C25" s="10">
+        <v>-2715.29541666667</v>
+      </c>
+      <c r="D25" s="10">
+        <v>-1267.3787500000001</v>
+      </c>
+      <c r="E25" s="10">
+        <v>-784.73986111111105</v>
+      </c>
+      <c r="F25" s="10">
+        <v>-543.42041666666705</v>
+      </c>
+      <c r="G25" s="10">
+        <v>-398.62875000000003</v>
+      </c>
+      <c r="H25" s="10">
+        <v>-302.10097222222203</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="18">
+        <v>-80000</v>
+      </c>
+      <c r="C26" s="18">
+        <v>-3637.9141666666701</v>
+      </c>
+      <c r="D26" s="18">
+        <v>-1742.08083333333</v>
+      </c>
+      <c r="E26" s="18">
+        <v>-1110.13638888889</v>
+      </c>
+      <c r="F26" s="18">
+        <v>-794.16416666666703</v>
+      </c>
+      <c r="G26" s="18">
+        <v>-604.58083333333298</v>
+      </c>
+      <c r="H26" s="18">
+        <v>-478.191944444444</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="10">
-        <v>-60000</v>
-      </c>
-      <c r="C21" s="10">
-        <v>-1792.6766666666699</v>
-      </c>
-      <c r="D21" s="10">
-        <v>-792.67666666666696</v>
-      </c>
-      <c r="E21" s="10">
-        <v>-459.34333333333302</v>
-      </c>
-      <c r="F21" s="10">
-        <v>-292.67666666666702</v>
-      </c>
-      <c r="G21" s="10">
-        <v>-192.67666666666699</v>
-      </c>
-      <c r="H21" s="10">
-        <v>-126.01</v>
-      </c>
-      <c r="J21" s="7">
-        <f>J19*120</f>
-        <v>35194.299999999996</v>
-      </c>
-      <c r="K21">
-        <f>60*B41</f>
-        <v>472.87614243637466</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="10">
-        <v>-70000</v>
-      </c>
-      <c r="C22" s="10">
-        <v>-2715.29541666667</v>
-      </c>
-      <c r="D22" s="10">
-        <v>-1267.3787500000001</v>
-      </c>
-      <c r="E22" s="10">
-        <v>-784.73986111111105</v>
-      </c>
-      <c r="F22" s="10">
-        <v>-543.42041666666705</v>
-      </c>
-      <c r="G22" s="10">
-        <v>-398.62875000000003</v>
-      </c>
-      <c r="H22" s="10">
-        <v>-302.10097222222203</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="18">
-        <v>-80000</v>
-      </c>
-      <c r="C23" s="18">
-        <v>-3637.9141666666701</v>
-      </c>
-      <c r="D23" s="18">
-        <v>-1742.08083333333</v>
-      </c>
-      <c r="E23" s="18">
-        <v>-1110.13638888889</v>
-      </c>
-      <c r="F23" s="18">
-        <v>-794.16416666666703</v>
-      </c>
-      <c r="G23" s="18">
-        <v>-604.58083333333298</v>
-      </c>
-      <c r="H23" s="18">
-        <v>-478.191944444444</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="B24" s="19">
+      <c r="B27" s="19">
         <f>E4</f>
         <v>-38.9652421246426</v>
       </c>
-      <c r="C24" s="20">
+      <c r="C27" s="20">
         <v>12</v>
       </c>
-      <c r="D24" s="20">
+      <c r="D27" s="20">
         <v>24</v>
       </c>
-      <c r="E24" s="20">
+      <c r="E27" s="20">
         <v>36</v>
       </c>
-      <c r="F24" s="20">
+      <c r="F27" s="20">
         <v>48</v>
       </c>
-      <c r="G24" s="20">
+      <c r="G27" s="20">
         <v>60</v>
       </c>
-      <c r="H24" s="20">
+      <c r="H27" s="20">
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>60</v>
-      </c>
-      <c r="B25" s="21">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="21">
         <v>0.03</v>
       </c>
-      <c r="C25" s="22">
+      <c r="C28" s="22">
         <v>-114.46875</v>
       </c>
-      <c r="D25" s="22">
+      <c r="D28" s="22">
         <v>-114.46875</v>
       </c>
-      <c r="E25" s="22">
+      <c r="E28" s="22">
         <v>-114.46875</v>
       </c>
-      <c r="F25" s="22">
+      <c r="F28" s="22">
         <v>-114.46875</v>
       </c>
-      <c r="G25" s="22">
+      <c r="G28" s="22">
         <v>-114.46875</v>
       </c>
-      <c r="H25" s="22">
+      <c r="H28" s="22">
         <v>-114.46875</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="23">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="C26" s="10">
-        <v>-133.546875</v>
-      </c>
-      <c r="D26" s="10">
-        <v>-133.546875</v>
-      </c>
-      <c r="E26" s="10">
-        <v>-133.546875</v>
-      </c>
-      <c r="F26" s="10">
-        <v>-133.546875</v>
-      </c>
-      <c r="G26" s="10">
-        <v>-133.546875</v>
-      </c>
-      <c r="H26" s="10">
-        <v>-133.546875</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="23">
-        <v>0.04</v>
-      </c>
-      <c r="C27" s="10">
-        <v>-152.625</v>
-      </c>
-      <c r="D27" s="10">
-        <v>-152.625</v>
-      </c>
-      <c r="E27" s="10">
-        <v>-152.625</v>
-      </c>
-      <c r="F27" s="10">
-        <v>-152.625</v>
-      </c>
-      <c r="G27" s="10">
-        <v>-152.625</v>
-      </c>
-      <c r="H27" s="10">
-        <v>-152.625</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="23">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="C28" s="10">
-        <v>-171.703125</v>
-      </c>
-      <c r="D28" s="10">
-        <v>-171.703125</v>
-      </c>
-      <c r="E28" s="10">
-        <v>-171.703125</v>
-      </c>
-      <c r="F28" s="10">
-        <v>-171.703125</v>
-      </c>
-      <c r="G28" s="10">
-        <v>-171.703125</v>
-      </c>
-      <c r="H28" s="10">
-        <v>-171.703125</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B29" s="23">
-        <v>0.05</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="C29" s="10">
-        <v>-190.78125</v>
+        <v>-133.546875</v>
       </c>
       <c r="D29" s="10">
-        <v>-190.78125</v>
+        <v>-133.546875</v>
       </c>
       <c r="E29" s="10">
-        <v>-190.78125</v>
+        <v>-133.546875</v>
       </c>
       <c r="F29" s="10">
-        <v>-190.78125</v>
+        <v>-133.546875</v>
       </c>
       <c r="G29" s="10">
-        <v>-190.78125</v>
+        <v>-133.546875</v>
       </c>
       <c r="H29" s="10">
-        <v>-190.78125</v>
+        <v>-133.546875</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B30" s="23">
+        <v>0.04</v>
+      </c>
+      <c r="C30" s="10">
+        <v>-152.625</v>
+      </c>
+      <c r="D30" s="10">
+        <v>-152.625</v>
+      </c>
+      <c r="E30" s="10">
+        <v>-152.625</v>
+      </c>
+      <c r="F30" s="10">
+        <v>-152.625</v>
+      </c>
+      <c r="G30" s="10">
+        <v>-152.625</v>
+      </c>
+      <c r="H30" s="10">
+        <v>-152.625</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="23">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="C31" s="10">
+        <v>-171.703125</v>
+      </c>
+      <c r="D31" s="10">
+        <v>-171.703125</v>
+      </c>
+      <c r="E31" s="10">
+        <v>-171.703125</v>
+      </c>
+      <c r="F31" s="10">
+        <v>-171.703125</v>
+      </c>
+      <c r="G31" s="10">
+        <v>-171.703125</v>
+      </c>
+      <c r="H31" s="10">
+        <v>-171.703125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="23">
+        <v>0.05</v>
+      </c>
+      <c r="C32" s="10">
+        <v>-190.78125</v>
+      </c>
+      <c r="D32" s="10">
+        <v>-190.78125</v>
+      </c>
+      <c r="E32" s="10">
+        <v>-190.78125</v>
+      </c>
+      <c r="F32" s="10">
+        <v>-190.78125</v>
+      </c>
+      <c r="G32" s="10">
+        <v>-190.78125</v>
+      </c>
+      <c r="H32" s="10">
+        <v>-190.78125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="23">
         <v>5.5E-2</v>
       </c>
-      <c r="C30" s="10">
+      <c r="C33" s="10">
         <v>-209.859375</v>
       </c>
-      <c r="D30" s="10">
+      <c r="D33" s="10">
         <v>-209.859375</v>
       </c>
-      <c r="E30" s="10">
+      <c r="E33" s="10">
         <v>-209.859375</v>
       </c>
-      <c r="F30" s="10">
+      <c r="F33" s="10">
         <v>-209.859375</v>
       </c>
-      <c r="G30" s="10">
+      <c r="G33" s="10">
         <v>-209.859375</v>
       </c>
-      <c r="H30" s="10">
+      <c r="H33" s="10">
         <v>-209.859375</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="23">
+    <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="23">
         <v>0.06</v>
       </c>
-      <c r="C31" s="10">
+      <c r="C34" s="10">
         <v>-228.9375</v>
       </c>
-      <c r="D31" s="10">
+      <c r="D34" s="10">
         <v>-228.9375</v>
       </c>
-      <c r="E31" s="10">
+      <c r="E34" s="10">
         <v>-228.9375</v>
       </c>
-      <c r="F31" s="10">
+      <c r="F34" s="10">
         <v>-228.9375</v>
       </c>
-      <c r="G31" s="10">
+      <c r="G34" s="10">
         <v>-228.9375</v>
       </c>
-      <c r="H31" s="10">
+      <c r="H34" s="10">
         <v>-228.9375</v>
       </c>
     </row>
-    <row r="32" spans="1:11" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="B32" s="14">
+    <row r="35" spans="1:8" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B35" s="14">
         <f>-1*PMT(B2/12,B8,E2)</f>
         <v>-667.11454768019814</v>
       </c>
-      <c r="C32" s="15" t="s">
+      <c r="C35" s="15" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="5">
-        <f>B32</f>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="5">
+        <f>B35</f>
         <v>-667.11454768019814</v>
       </c>
-      <c r="C33" s="16">
+      <c r="C36" s="16">
         <v>12</v>
       </c>
-      <c r="D33" s="16">
+      <c r="D36" s="16">
         <v>24</v>
       </c>
-      <c r="E33" s="16">
+      <c r="E36" s="16">
         <v>36</v>
       </c>
-      <c r="F33" s="16">
+      <c r="F36" s="16">
         <v>48</v>
       </c>
-      <c r="G33" s="16">
+      <c r="G36" s="16">
         <v>60</v>
       </c>
-      <c r="H33" s="16">
+      <c r="H36" s="16">
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="10">
+      <c r="B37" s="10">
         <v>-40000</v>
       </c>
-      <c r="C34" s="10">
+      <c r="C37" s="10">
         <v>-1115.7249999999999</v>
       </c>
-      <c r="D34" s="10">
+      <c r="D37" s="10">
         <v>-574.05833333333305</v>
       </c>
-      <c r="E34" s="10">
+      <c r="E37" s="10">
         <v>-393.50277777777802</v>
       </c>
-      <c r="F34" s="10">
+      <c r="F37" s="10">
         <v>-303.22500000000002</v>
       </c>
-      <c r="G34" s="10">
+      <c r="G37" s="10">
         <v>-249.058333333333</v>
       </c>
-      <c r="H34" s="10">
+      <c r="H37" s="10">
         <v>-212.947222222222</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="10">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="10">
         <v>-50000</v>
       </c>
-      <c r="C35" s="10">
+      <c r="C38" s="10">
         <v>-2038.34375</v>
       </c>
-      <c r="D35" s="10">
+      <c r="D38" s="10">
         <v>-1048.7604166666699</v>
       </c>
-      <c r="E35" s="10">
+      <c r="E38" s="10">
         <v>-718.899305555556</v>
       </c>
-      <c r="F35" s="10">
+      <c r="F38" s="10">
         <v>-553.96875</v>
       </c>
-      <c r="G35" s="10">
+      <c r="G38" s="10">
         <v>-455.01041666666703</v>
       </c>
-      <c r="H35" s="10">
+      <c r="H38" s="10">
         <v>-389.038194444444</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="10">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="10">
         <v>-60000</v>
       </c>
-      <c r="C36" s="10">
+      <c r="C39" s="10">
         <v>-2960.9625000000001</v>
       </c>
-      <c r="D36" s="10">
+      <c r="D39" s="10">
         <v>-1523.4625000000001</v>
       </c>
-      <c r="E36" s="10">
+      <c r="E39" s="10">
         <v>-1044.2958333333299</v>
       </c>
-      <c r="F36" s="10">
+      <c r="F39" s="10">
         <v>-804.71249999999998</v>
       </c>
-      <c r="G36" s="10">
+      <c r="G39" s="10">
         <v>-660.96249999999998</v>
       </c>
-      <c r="H36" s="10">
+      <c r="H39" s="10">
         <v>-565.12916666666695</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="10">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="10">
         <v>-70000</v>
       </c>
-      <c r="C37" s="10">
+      <c r="C40" s="10">
         <v>-3883.5812500000002</v>
       </c>
-      <c r="D37" s="10">
+      <c r="D40" s="10">
         <v>-1998.16458333333</v>
       </c>
-      <c r="E37" s="10">
+      <c r="E40" s="10">
         <v>-1369.6923611111099</v>
       </c>
-      <c r="F37" s="10">
+      <c r="F40" s="10">
         <v>-1055.45625</v>
       </c>
-      <c r="G37" s="10">
+      <c r="G40" s="10">
         <v>-866.91458333333298</v>
       </c>
-      <c r="H37" s="10">
+      <c r="H40" s="10">
         <v>-741.22013888888898</v>
       </c>
     </row>
-    <row r="38" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="18">
+    <row r="41" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="18">
         <v>-80000</v>
       </c>
-      <c r="C38" s="10">
+      <c r="C41" s="10">
         <v>-4806.2</v>
       </c>
-      <c r="D38" s="18">
+      <c r="D41" s="18">
         <v>-2472.86666666667</v>
       </c>
-      <c r="E38" s="18">
+      <c r="E41" s="18">
         <v>-1695.0888888888901</v>
       </c>
-      <c r="F38" s="18">
+      <c r="F41" s="18">
         <v>-1306.2</v>
       </c>
-      <c r="G38" s="18">
+      <c r="G41" s="18">
         <v>-1072.86666666667</v>
       </c>
-      <c r="H38" s="18">
+      <c r="H41" s="18">
         <v>-917.31111111111102</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>61</v>
-      </c>
-      <c r="B39">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>60</v>
+      </c>
+      <c r="B42">
         <f>Q2</f>
         <v>600.82026666666673</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>61</v>
+      </c>
+      <c r="B43">
+        <v>5.95</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>62</v>
       </c>
-      <c r="B40">
-        <v>5.95</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>63</v>
-      </c>
-      <c r="B41">
-        <f>(B40/1000)*(1000/453.592)*B39</f>
+      <c r="B44">
+        <f>(B43/1000)*(1000/453.592)*B42</f>
         <v>7.8812690406062442</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F44">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F47">
         <v>53000</v>
       </c>
-      <c r="G44">
-        <v>70000</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F45">
+      <c r="G47">
+        <v>67000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F48">
         <v>32000</v>
       </c>
-      <c r="G45">
+      <c r="G48">
         <v>100000</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G46">
-        <f>(G44*F44)+(G45*F45)</f>
-        <v>6910000000</v>
+    <row r="49" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G49">
+        <f>(G47*F47)+(G48*F48)</f>
+        <v>6751000000</v>
       </c>
     </row>
   </sheetData>
@@ -4537,10 +4670,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U58"/>
+  <dimension ref="A1:U62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4571,39 +4704,39 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" t="s">
         <v>65</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>66</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>67</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>68</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>69</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>70</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>71</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>72</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>73</v>
-      </c>
-      <c r="K2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -4611,28 +4744,28 @@
         <v>-35000</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D3">
         <v>-9000</v>
       </c>
       <c r="E3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" t="s">
         <v>76</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>77</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" t="s">
         <v>78</v>
-      </c>
-      <c r="H3" t="s">
-        <v>75</v>
-      </c>
-      <c r="I3" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -4708,45 +4841,45 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" t="s">
         <v>80</v>
-      </c>
-      <c r="B8" t="s">
-        <v>81</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
       <c r="F8" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H8" t="s">
+        <v>159</v>
+      </c>
+      <c r="I8" s="39" t="s">
         <v>160</v>
       </c>
-      <c r="I8" s="39" t="s">
-        <v>161</v>
-      </c>
       <c r="J8" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="K8" s="39" t="s">
+        <v>153</v>
+      </c>
+      <c r="L8" t="s">
         <v>152</v>
-      </c>
-      <c r="K8" s="39" t="s">
-        <v>154</v>
-      </c>
-      <c r="L8" t="s">
-        <v>153</v>
       </c>
       <c r="M8" s="12">
         <f>SUMIF(J:J,"Performance",F:F)</f>
-        <v>-3739.6800000000003</v>
+        <v>-3348.2200000000003</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D9" s="12">
         <v>-3100</v>
@@ -4755,7 +4888,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="12">
-        <f t="shared" ref="F9:H43" si="1">IF(E9=1,D9,0)</f>
+        <f t="shared" ref="F9:H44" si="1">IF(E9=1,D9,0)</f>
         <v>0</v>
       </c>
       <c r="G9">
@@ -4770,13 +4903,13 @@
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M9" s="12">
         <f>SUMIF(J:J,"Aesthetic",F:F)</f>
@@ -4787,7 +4920,7 @@
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D10" s="12">
         <v>-300</v>
@@ -4807,26 +4940,26 @@
         <v>0</v>
       </c>
       <c r="I10" s="12">
-        <f t="shared" ref="I10:I43" si="2">IF(G10=2,F10,0)</f>
+        <f t="shared" ref="I10:I44" si="2">IF(G10=2,F10,0)</f>
         <v>0</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K10" t="s">
+        <v>154</v>
+      </c>
+      <c r="L10" t="s">
         <v>155</v>
-      </c>
-      <c r="L10" t="s">
-        <v>156</v>
       </c>
       <c r="M10" s="12">
         <f>SUMIF(J:J,"Comfort",F:F)</f>
-        <v>0</v>
+        <v>-150</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D11" s="12">
         <v>-1200</v>
@@ -4850,20 +4983,20 @@
         <v>0</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K11" s="11"/>
       <c r="L11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M11" s="12">
         <f>SUMIF(J:J,"Maintenance",F:F)</f>
-        <v>-1462</v>
+        <v>-1276</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D12" s="12">
         <v>-1500</v>
@@ -4887,13 +5020,13 @@
         <v>0</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M12" s="12">
         <f>SUMIF(J:J,"Functionality",F:F)</f>
@@ -4910,7 +5043,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D13" s="12">
         <v>-2500</v>
@@ -4934,15 +5067,15 @@
         <v>0</v>
       </c>
       <c r="J13" s="40" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D14" s="12">
         <v>-1200</v>
@@ -4966,15 +5099,15 @@
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D15" s="12">
         <v>-500</v>
@@ -4998,15 +5131,15 @@
         <v>0</v>
       </c>
       <c r="J15" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D16" s="12">
         <v>-500</v>
@@ -5030,15 +5163,15 @@
         <v>0</v>
       </c>
       <c r="J16" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D17" s="12">
         <v>-800</v>
@@ -5062,15 +5195,15 @@
         <v>0</v>
       </c>
       <c r="J17" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D18" s="12">
         <v>-2250</v>
@@ -5094,15 +5227,15 @@
         <v>0</v>
       </c>
       <c r="J18" s="39" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D19" s="12">
         <v>-2500</v>
@@ -5126,15 +5259,15 @@
         <v>0</v>
       </c>
       <c r="J19" s="39" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K19" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D20" s="12">
         <v>-1000</v>
@@ -5158,15 +5291,15 @@
         <v>0</v>
       </c>
       <c r="J20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D21" s="12">
         <v>-1750.26</v>
@@ -5190,18 +5323,18 @@
         <v>0</v>
       </c>
       <c r="J21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K21" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C22" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D22" s="12">
         <v>-1233.06</v>
@@ -5224,50 +5357,50 @@
         <v>0</v>
       </c>
       <c r="J22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D23" s="12">
-        <v>-691.46</v>
+        <v>-300</v>
       </c>
       <c r="E23" s="11">
         <v>1</v>
       </c>
       <c r="F23" s="12">
         <f t="shared" si="1"/>
-        <v>-691.46</v>
+        <v>-300</v>
       </c>
       <c r="G23">
         <v>1</v>
       </c>
       <c r="H23" s="12">
         <f t="shared" si="1"/>
-        <v>-691.46</v>
+        <v>-300</v>
       </c>
       <c r="I23" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D24" s="12">
         <v>-350</v>
@@ -5291,15 +5424,15 @@
         <v>0</v>
       </c>
       <c r="J24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D25" s="12">
         <v>-1380</v>
@@ -5323,15 +5456,15 @@
         <v>0</v>
       </c>
       <c r="J25" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D26" s="12">
         <v>-427.66</v>
@@ -5355,15 +5488,15 @@
         <v>0</v>
       </c>
       <c r="J26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D27" s="12">
         <v>-900</v>
@@ -5387,18 +5520,18 @@
         <v>0</v>
       </c>
       <c r="J27" s="39" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K27" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
+        <v>109</v>
+      </c>
+      <c r="C28" t="s">
         <v>110</v>
-      </c>
-      <c r="C28" t="s">
-        <v>111</v>
       </c>
       <c r="D28" s="12">
         <v>-1700</v>
@@ -5422,15 +5555,15 @@
         <v>0</v>
       </c>
       <c r="J28" s="39" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K28" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D29" s="12">
         <v>-550</v>
@@ -5454,18 +5587,18 @@
         <v>0</v>
       </c>
       <c r="J29" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C30" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D30" s="12">
         <v>-30</v>
@@ -5489,21 +5622,21 @@
         <v>0</v>
       </c>
       <c r="J30" s="39" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K30" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B31" t="s">
+        <v>126</v>
+      </c>
+      <c r="C31" t="s">
         <v>127</v>
-      </c>
-      <c r="C31" t="s">
-        <v>128</v>
       </c>
       <c r="D31" s="12">
         <v>-100</v>
@@ -5527,12 +5660,12 @@
         <v>0</v>
       </c>
       <c r="J31" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D32" s="12">
         <v>-16</v>
@@ -5556,12 +5689,12 @@
         <v>0</v>
       </c>
       <c r="J32" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D33" s="12">
         <v>-12</v>
@@ -5585,12 +5718,12 @@
         <v>0</v>
       </c>
       <c r="J33" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D34" s="12">
         <v>-46</v>
@@ -5614,52 +5747,49 @@
         <v>0</v>
       </c>
       <c r="J34" s="39" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>126</v>
-      </c>
       <c r="C35" t="s">
-        <v>132</v>
+        <v>186</v>
       </c>
       <c r="D35" s="12">
+        <v>-18</v>
+      </c>
+      <c r="E35" s="11">
+        <v>0</v>
+      </c>
+      <c r="F35" s="12">
+        <f t="shared" ref="F35" si="3">IF(E35=1,D35,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35" s="12">
+        <f t="shared" ref="H35" si="4">IF(G35=1,F35,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I35" s="12">
+        <f t="shared" ref="I35" si="5">IF(G35=2,F35,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J35" s="39" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>125</v>
+      </c>
+      <c r="C36" t="s">
+        <v>131</v>
+      </c>
+      <c r="D36" s="12">
         <v>-30</v>
       </c>
-      <c r="E35" s="11">
-        <v>0</v>
-      </c>
-      <c r="F35" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G35">
-        <v>0</v>
-      </c>
-      <c r="H35" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I35" s="12">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J35" t="s">
-        <v>155</v>
-      </c>
-      <c r="K35" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>139</v>
-      </c>
-      <c r="D36" s="12">
-        <v>-18</v>
-      </c>
-      <c r="E36" s="40">
+      <c r="E36" s="11">
         <v>0</v>
       </c>
       <c r="F36" s="12">
@@ -5677,21 +5807,21 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J36" s="39" t="s">
-        <v>157</v>
+      <c r="J36" t="s">
+        <v>154</v>
+      </c>
+      <c r="K36" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>138</v>
       </c>
-      <c r="C37" t="s">
-        <v>137</v>
-      </c>
-      <c r="D37" s="39">
-        <v>-29</v>
-      </c>
-      <c r="E37">
+      <c r="D37" s="12">
+        <v>-18</v>
+      </c>
+      <c r="E37" s="40">
         <v>0</v>
       </c>
       <c r="F37" s="12">
@@ -5709,19 +5839,19 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J37" s="12" t="s">
+      <c r="J37" s="39" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>171</v>
+        <v>137</v>
       </c>
       <c r="C38" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D38" s="39">
-        <v>-100</v>
+        <v>-29</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -5742,50 +5872,50 @@
         <v>0</v>
       </c>
       <c r="J38" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>145</v>
+        <v>181</v>
       </c>
       <c r="C39" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D39" s="39">
-        <v>-15</v>
+        <v>-150</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F39" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-150</v>
       </c>
       <c r="G39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H39" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-150</v>
       </c>
       <c r="I39" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J39" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C40" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D40" s="39">
-        <v>-20</v>
+        <v>-15</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -5805,19 +5935,19 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J40" t="s">
+      <c r="J40" s="12" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C41" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D41" s="39">
-        <v>-440</v>
+        <v>-20</v>
       </c>
       <c r="E41">
         <v>0</v>
@@ -5837,19 +5967,19 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J41" s="39" t="s">
-        <v>159</v>
+      <c r="J41" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C42" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D42" s="39">
-        <v>-95</v>
+        <v>-440</v>
       </c>
       <c r="E42">
         <v>0</v>
@@ -5875,164 +6005,167 @@
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="C43" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="D43" s="39">
-        <v>-25</v>
+        <v>-95</v>
       </c>
       <c r="E43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F43" s="12">
         <f t="shared" si="1"/>
-        <v>-25</v>
+        <v>0</v>
       </c>
       <c r="G43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H43" s="12">
         <f t="shared" si="1"/>
-        <v>-25</v>
+        <v>0</v>
       </c>
       <c r="I43" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J43" s="39" t="s">
-        <v>180</v>
+        <v>157</v>
       </c>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="C44" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="D44" s="39">
-        <v>-100</v>
+        <v>-25</v>
       </c>
       <c r="E44">
         <v>1</v>
       </c>
       <c r="F44" s="12">
-        <f t="shared" ref="F44" si="3">IF(E44=1,D44,0)</f>
-        <v>-100</v>
+        <f t="shared" si="1"/>
+        <v>-25</v>
       </c>
       <c r="G44">
         <v>1</v>
       </c>
       <c r="H44" s="12">
-        <f t="shared" ref="H44" si="4">IF(G44=1,F44,0)</f>
-        <v>-100</v>
+        <f t="shared" si="1"/>
+        <v>-25</v>
       </c>
       <c r="I44" s="12">
-        <f t="shared" ref="I44" si="5">IF(G44=2,F44,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J44" s="39" t="s">
-        <v>157</v>
+        <v>178</v>
       </c>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="C45" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="D45" s="39">
-        <v>-330</v>
+        <v>-100</v>
       </c>
       <c r="E45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F45" s="12">
         <f t="shared" ref="F45" si="6">IF(E45=1,D45,0)</f>
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="G45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H45" s="12">
         <f t="shared" ref="H45" si="7">IF(G45=1,F45,0)</f>
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="I45" s="12">
         <f t="shared" ref="I45" si="8">IF(G45=2,F45,0)</f>
         <v>0</v>
       </c>
       <c r="J45" s="39" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>176</v>
+      </c>
       <c r="C46" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D46" s="39">
+        <v>-330</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46" s="12">
+        <f t="shared" ref="F46" si="9">IF(E46=1,D46,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46" s="12">
+        <f t="shared" ref="H46" si="10">IF(G46=1,F46,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I46" s="12">
+        <f t="shared" ref="I46" si="11">IF(G46=2,F46,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J46" s="39" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>173</v>
+      </c>
+      <c r="D47" s="39">
         <v>-186</v>
       </c>
-      <c r="E46">
-        <v>1</v>
-      </c>
-      <c r="F46" s="12">
-        <f t="shared" ref="F46:F48" si="9">IF(E46=1,D46,0)</f>
-        <v>-186</v>
-      </c>
-      <c r="G46">
-        <v>0</v>
-      </c>
-      <c r="H46" s="12">
-        <f t="shared" ref="H46:H48" si="10">IF(G46=1,F46,0)</f>
-        <v>0</v>
-      </c>
-      <c r="I46" s="12">
-        <f t="shared" ref="I46:I48" si="11">IF(G46=2,F46,0)</f>
-        <v>0</v>
-      </c>
-      <c r="J46" s="39" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>181</v>
-      </c>
-      <c r="C47" t="s">
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47" s="12">
+        <f t="shared" ref="F47:F52" si="12">IF(E47=1,D47,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47" s="12">
+        <f t="shared" ref="H47:H52" si="13">IF(G47=1,F47,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I47" s="12">
+        <f t="shared" ref="I47:I52" si="14">IF(G47=2,F47,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J47" s="39" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
         <v>179</v>
       </c>
-      <c r="D47" s="39">
-        <v>-100</v>
-      </c>
-      <c r="E47">
-        <v>1</v>
-      </c>
-      <c r="F47" s="12">
-        <f t="shared" si="9"/>
-        <v>-100</v>
-      </c>
-      <c r="G47">
-        <v>0</v>
-      </c>
-      <c r="H47" s="12">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="I47" s="12">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="J47" s="39" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D48" s="39">
         <v>-100</v>
@@ -6041,72 +6174,193 @@
         <v>1</v>
       </c>
       <c r="F48" s="12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>-100</v>
       </c>
       <c r="G48">
         <v>0</v>
       </c>
       <c r="H48" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="I48" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="J48" s="39" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
-        <v>74</v>
-      </c>
-      <c r="D49" s="12"/>
+        <v>185</v>
+      </c>
+      <c r="D49" s="39">
+        <v>-400</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
       <c r="F49" s="12">
-        <f>SUM(F9:F48)</f>
-        <v>-5226.68</v>
+        <f t="shared" si="12"/>
+        <v>-400</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
       </c>
       <c r="H49" s="12">
-        <f>SUM(H9:H48)</f>
-        <v>-4840.68</v>
+        <f t="shared" si="13"/>
+        <v>0</v>
       </c>
       <c r="I49" s="12">
-        <f>SUM(I9:I40)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>178</v>
-      </c>
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="J49" s="39"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>180</v>
+      </c>
+      <c r="D50" s="39">
+        <v>-100</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50" s="12">
+        <f t="shared" si="12"/>
+        <v>-100</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50" s="12">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="I50" s="12">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="J50" s="39" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
+        <v>125</v>
+      </c>
+      <c r="C51" t="s">
+        <v>182</v>
+      </c>
+      <c r="D51" s="39">
+        <v>-27</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51" s="12">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51" s="12">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="I51" s="12">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="J51" s="39" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>184</v>
+      </c>
+      <c r="C52" t="s">
+        <v>183</v>
+      </c>
+      <c r="D52" s="39">
+        <f>-205+-140</f>
+        <v>-345</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52" s="12">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52" s="12">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="I52" s="12">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="J52" s="39" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>73</v>
+      </c>
+      <c r="D53" s="12"/>
+      <c r="F53" s="12">
+        <f>SUM(F9:F52)</f>
+        <v>-5199.22</v>
+      </c>
+      <c r="H53" s="12">
+        <f>SUM(H9:H52)</f>
+        <v>-4599.22</v>
+      </c>
+      <c r="I53" s="12">
+        <f>SUM(I9:I41)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>176</v>
+      </c>
+      <c r="B55" t="s">
+        <v>173</v>
+      </c>
+      <c r="C55">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>174</v>
+      </c>
+      <c r="C56" s="12">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
         <v>175</v>
       </c>
-      <c r="C51">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>176</v>
-      </c>
-      <c r="C52" s="12">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>177</v>
-      </c>
-      <c r="C53">
+      <c r="C57">
         <v>280</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F58">
-        <f>SUM(F56:F57)</f>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F62">
+        <f>SUM(F60:F61)</f>
         <v>0</v>
       </c>
     </row>
@@ -6135,7 +6389,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6147,12 +6401,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D2">
         <f>-1*93*12</f>
@@ -6161,10 +6415,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" t="s">
         <v>115</v>
-      </c>
-      <c r="B3" t="s">
-        <v>116</v>
       </c>
       <c r="C3">
         <v>-1453.8</v>
@@ -6176,30 +6430,30 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C8">
         <v>-1902</v>
@@ -6211,48 +6465,58 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C15">
-        <f>900.4*2</f>
-        <v>1800.8</v>
+        <f>-900.4*2</f>
+        <v>-1800.8</v>
       </c>
       <c r="D15">
-        <f>726.9*2</f>
-        <v>1453.8</v>
+        <f>-726.9*2</f>
+        <v>-1453.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <f>C15/12</f>
+        <v>-150.06666666666666</v>
+      </c>
+      <c r="D16">
+        <f>D15/12</f>
+        <v>-121.14999999999999</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D17" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -6274,26 +6538,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" t="s">
         <v>104</v>
-      </c>
-      <c r="B1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" t="s">
         <v>106</v>
-      </c>
-      <c r="B3" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" t="s">
         <v>108</v>
-      </c>
-      <c r="B5" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>